<commit_message>
3/2 is now a Tu schedule
</commit_message>
<xml_diff>
--- a/ADMIN/S26 IDM Syllabus.xlsx
+++ b/ADMIN/S26 IDM Syllabus.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8440DFE0-1E29-44D7-A33D-E6D4DA2B4B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{8440DFE0-1E29-44D7-A33D-E6D4DA2B4B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A72509A4-DAD5-42E2-BAB3-FA3F68D2E7CF}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>PuLP</t>
   </si>
   <si>
-    <t>Midterm Exam, Part I</t>
-  </si>
-  <si>
     <t>Transshipment Problem</t>
   </si>
   <si>
@@ -196,6 +193,31 @@
       </rPr>
       <t xml:space="preserve">
 Midterm Exam, Part II</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">MON 2-MAR is a TU schedule
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Midterm Exam, Part I</t>
     </r>
   </si>
 </sst>
@@ -292,12 +314,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -350,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,13 +398,17 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -664,8 +696,8 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>8</v>
@@ -703,10 +735,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
@@ -721,7 +753,7 @@
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="14">
         <f>B2+2</f>
@@ -744,17 +776,17 @@
         <v>14</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="15">
         <f t="shared" ref="F3:F16" si="0">B3+2</f>
         <v>46044</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="10"/>
     </row>
@@ -767,20 +799,20 @@
         <v>46049</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="15">
         <f t="shared" si="0"/>
         <v>46051</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="10"/>
     </row>
@@ -793,20 +825,20 @@
         <v>46056</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="F5" s="15">
         <f t="shared" si="0"/>
         <v>46058</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="10"/>
     </row>
@@ -819,20 +851,20 @@
         <v>46063</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="F6" s="15">
         <f t="shared" si="0"/>
         <v>46065</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="10"/>
     </row>
@@ -845,20 +877,20 @@
         <v>46070</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="15">
         <f t="shared" si="0"/>
         <v>46072</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
@@ -870,7 +902,7 @@
         <v>46077</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="12"/>
@@ -882,7 +914,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="10"/>
     </row>
@@ -890,27 +922,26 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="9">
-        <f t="shared" si="1"/>
-        <v>46084</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
+      <c r="B9" s="20">
+        <v>46083</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="10"/>
       <c r="F9" s="15">
         <v>45720</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>38</v>
+      <c r="G9" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="9">
-        <f t="shared" si="1"/>
+        <f>B8+14</f>
         <v>46091</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -940,7 +971,7 @@
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="15">
         <f t="shared" si="0"/>
@@ -962,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="15">
         <f t="shared" si="0"/>
@@ -988,10 +1019,10 @@
         <v>11</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="F13" s="15">
         <f t="shared" si="0"/>
@@ -1014,10 +1045,10 @@
         <v>6</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>32</v>
       </c>
       <c r="F14" s="15">
         <f t="shared" si="0"/>
@@ -1040,10 +1071,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="F15" s="15">
         <f t="shared" si="0"/>
@@ -1066,10 +1097,10 @@
         <v>7</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="F16" s="15">
         <f t="shared" si="0"/>
@@ -1089,17 +1120,17 @@
         <v>46140</v>
       </c>
       <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>

</xml_diff>

<commit_message>
updated lec09-10 part II slides, updated syllabus
</commit_message>
<xml_diff>
--- a/ADMIN/S26 IDM Syllabus.xlsx
+++ b/ADMIN/S26 IDM Syllabus.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{8440DFE0-1E29-44D7-A33D-E6D4DA2B4B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A72509A4-DAD5-42E2-BAB3-FA3F68D2E7CF}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{8440DFE0-1E29-44D7-A33D-E6D4DA2B4B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{268A782B-53D2-4275-860A-C0736D86DABF}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Tu</t>
   </si>
@@ -220,6 +220,13 @@
       <t>Midterm Exam, Part I</t>
     </r>
   </si>
+  <si>
+    <t>Stable Marriage Problem / 
+Sports Scheduling Problem</t>
+  </si>
+  <si>
+    <t>HW 6^</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,15 +304,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="14"/>
       <color theme="1"/>
@@ -313,19 +311,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -378,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -397,7 +404,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -407,8 +413,10 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -696,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,13 +891,13 @@
         <f t="shared" si="0"/>
         <v>46072</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -904,8 +912,12 @@
       <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="F8" s="15">
         <f t="shared" si="0"/>
         <v>46079</v>
@@ -913,7 +925,7 @@
       <c r="G8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="20" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="10"/>
@@ -922,10 +934,10 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="21">
         <v>46083</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="8"/>
@@ -933,7 +945,7 @@
       <c r="F9" s="15">
         <v>45720</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>37</v>
       </c>
       <c r="H9" s="10"/>
@@ -969,7 +981,9 @@
       <c r="C11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1126,11 +1140,11 @@
         <v>33</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
@@ -1159,7 +1173,7 @@
     <oddHeader>&amp;C&amp;"-,Bold"&amp;14
 Intermediate Deterministic Models&amp;R
 &amp;9 SPRING 2026</oddHeader>
-    <oddFooter>&amp;C&amp;"-,Bold"&amp;13*HW is due at the beginning of class on the day it is due.&amp;"-,Regular"&amp;11
+    <oddFooter>&amp;C&amp;"-,Bold"&amp;13*HW is due at the beginning of class on the day it is due.   &amp;K00B0F0 ^ HW 6 material will be on the midterm exam.&amp;"-,Regular"&amp;11&amp;K01+000
  Syllabus subject to change; updates will be posted on GitHub.</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>